<commit_message>
backplane bom filled in
</commit_message>
<xml_diff>
--- a/hardware/backplane/rev_a/backplane_bom.xlsx
+++ b/hardware/backplane/rev_a/backplane_bom.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="131">
   <si>
     <t>Qty</t>
   </si>
@@ -415,6 +415,33 @@
   </si>
   <si>
     <t>490-5868-1-ND</t>
+  </si>
+  <si>
+    <t>0603 Capacitor</t>
+  </si>
+  <si>
+    <t>1210 Capacitor</t>
+  </si>
+  <si>
+    <t>490-10477-1-ND</t>
+  </si>
+  <si>
+    <t>RHM27CECT-ND</t>
+  </si>
+  <si>
+    <t>RHM49.9CFCT-ND</t>
+  </si>
+  <si>
+    <t>RHM1.50KHCT-ND</t>
+  </si>
+  <si>
+    <t>RHM10.0KHCT-ND</t>
+  </si>
+  <si>
+    <t>RHM15.0KCFCT-ND</t>
+  </si>
+  <si>
+    <t>RHM10MDCT-ND</t>
   </si>
 </sst>
 </file>
@@ -487,8 +514,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -500,9 +529,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -785,7 +816,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -837,7 +868,7 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="G2" t="s">
         <v>31</v>
@@ -883,7 +914,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>120</v>
@@ -906,7 +937,10 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>122</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -926,7 +960,7 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>123</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -1086,6 +1120,9 @@
       <c r="F13" t="s">
         <v>10</v>
       </c>
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1106,6 +1143,9 @@
       <c r="F14" t="s">
         <v>10</v>
       </c>
+      <c r="G14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1126,6 +1166,9 @@
       <c r="F15" t="s">
         <v>10</v>
       </c>
+      <c r="G15" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1146,6 +1189,9 @@
       <c r="F16" t="s">
         <v>10</v>
       </c>
+      <c r="G16" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1166,6 +1212,9 @@
       <c r="F17" t="s">
         <v>10</v>
       </c>
+      <c r="G17" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1186,6 +1235,9 @@
       <c r="F18" t="s">
         <v>10</v>
       </c>
+      <c r="G18" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1235,45 +1287,45 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" s="3" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>6</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1347,25 +1399,25 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="G26" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1373,45 +1425,45 @@
         <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="E27" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="G28" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>